<commit_message>
feat: add reminder value for BarChart
</commit_message>
<xml_diff>
--- a/server/public/downloads/Гос. задание 2026.xlsx
+++ b/server/public/downloads/Гос. задание 2026.xlsx
@@ -1427,15 +1427,15 @@
       </c>
       <c r="C3" s="7">
         <f>ППК!K5</f>
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="D3" s="7">
         <f t="shared" ref="D3:D6" si="0">C3/B3*100</f>
-        <v>9.5233741695617731</v>
+        <v>0</v>
       </c>
       <c r="E3" s="7">
         <f t="shared" ref="E3:E6" si="1">B3-C3</f>
-        <v>47502.400000000001</v>
+        <v>52502.400000000001</v>
       </c>
     </row>
     <row r="4" ht="30" customHeight="1">
@@ -1651,7 +1651,7 @@
       </c>
       <c r="K5" s="18">
         <f>G37+G75+G113+G151+G189</f>
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="L5" s="10"/>
     </row>
@@ -1673,7 +1673,7 @@
       </c>
       <c r="K6" s="22">
         <f>K5/K4*100</f>
-        <v>8.5710367526055951</v>
+        <v>0</v>
       </c>
       <c r="L6" s="10"/>
     </row>
@@ -1695,7 +1695,7 @@
       </c>
       <c r="K7" s="18">
         <f>K4-K5</f>
-        <v>53336</v>
+        <v>58336</v>
       </c>
       <c r="L7" s="10"/>
     </row>
@@ -1704,15 +1704,11 @@
       <c r="B8" s="19"/>
       <c r="C8" s="20"/>
       <c r="D8" s="20"/>
-      <c r="E8" s="19">
-        <v>1000</v>
-      </c>
-      <c r="F8" s="19">
-        <v>5</v>
-      </c>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
       <c r="G8" s="12">
         <f t="shared" si="2"/>
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="H8" s="21"/>
       <c r="I8" s="10"/>
@@ -2296,15 +2292,15 @@
       </c>
       <c r="E37" s="40">
         <f>SUM(E3:E36)</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F37" s="40">
         <f>SUM(F3:F36)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G37" s="41">
         <f>SUM(G3:G36)</f>
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="H37" s="38"/>
       <c r="I37" s="10"/>

</xml_diff>